<commit_message>
Notebook updates and field standardization to have corresponding column names across ground truth datasets
</commit_message>
<xml_diff>
--- a/output/gold/GT_DataLinks_PMC_and_Fenyo.xlsx
+++ b/output/gold/GT_DataLinks_PMC_and_Fenyo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pietro/Desktop/VIDA-NYU/data-gatherer/output/gold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFB9D17-2E71-834A-A6B8-5CE42666FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB7D61-6427-F04A-A660-3F63B2BB69F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Links Ground Truth" sheetId="3" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>PXD047284</t>
   </si>
   <si>
-    <t>Source Page</t>
-  </si>
-  <si>
-    <t>UID</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC11252349/</t>
   </si>
   <si>
@@ -462,13 +456,19 @@
     <t>MSV000092944</t>
   </si>
   <si>
-    <t>Dataset Webpage</t>
-  </si>
-  <si>
-    <t>Repository Link</t>
-  </si>
-  <si>
-    <t>Repo Name</t>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>repository</t>
+  </si>
+  <si>
+    <t>citing_publication_link</t>
+  </si>
+  <si>
+    <t>repo_link</t>
+  </si>
+  <si>
+    <t>dataset_webpage</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -833,19 +833,19 @@
   <sheetData>
     <row r="1" spans="1:134" ht="32.25" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -979,19 +979,19 @@
     </row>
     <row r="2" spans="1:134" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1044,19 +1044,19 @@
     </row>
     <row r="3" spans="1:134" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1109,19 +1109,19 @@
     </row>
     <row r="4" spans="1:134" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -1174,19 +1174,19 @@
     </row>
     <row r="5" spans="1:134" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
@@ -1239,19 +1239,19 @@
     </row>
     <row r="6" spans="1:134" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -1304,19 +1304,19 @@
     </row>
     <row r="7" spans="1:134" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
@@ -1369,19 +1369,19 @@
     </row>
     <row r="8" spans="1:134" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -1434,19 +1434,19 @@
     </row>
     <row r="9" spans="1:134" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
@@ -1499,19 +1499,19 @@
     </row>
     <row r="10" spans="1:134" ht="15.75" customHeight="1">
       <c r="A10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>
@@ -1564,19 +1564,19 @@
     </row>
     <row r="11" spans="1:134" ht="16">
       <c r="A11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="4"/>
@@ -1709,19 +1709,19 @@
     </row>
     <row r="12" spans="1:134" ht="16">
       <c r="A12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -1854,19 +1854,19 @@
     </row>
     <row r="13" spans="1:134" ht="16">
       <c r="A13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
@@ -1999,19 +1999,19 @@
     </row>
     <row r="14" spans="1:134" ht="16">
       <c r="A14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4"/>
@@ -2144,19 +2144,19 @@
     </row>
     <row r="15" spans="1:134" ht="16">
       <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="4"/>
@@ -2289,19 +2289,19 @@
     </row>
     <row r="16" spans="1:134" ht="16">
       <c r="A16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="4"/>
@@ -2434,19 +2434,19 @@
     </row>
     <row r="17" spans="1:134" ht="16">
       <c r="A17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="4"/>
@@ -2579,19 +2579,19 @@
     </row>
     <row r="18" spans="1:134" ht="16">
       <c r="A18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="4"/>
@@ -2724,19 +2724,19 @@
     </row>
     <row r="19" spans="1:134" ht="16">
       <c r="A19" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="4"/>
@@ -2869,19 +2869,19 @@
     </row>
     <row r="20" spans="1:134" ht="16">
       <c r="A20" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="4"/>
@@ -3014,19 +3014,19 @@
     </row>
     <row r="21" spans="1:134" ht="16">
       <c r="A21" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="4"/>
@@ -3159,19 +3159,19 @@
     </row>
     <row r="22" spans="1:134" ht="16">
       <c r="A22" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -3304,19 +3304,19 @@
     </row>
     <row r="23" spans="1:134" ht="15.75" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -3369,19 +3369,19 @@
     </row>
     <row r="24" spans="1:134" ht="15.75" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
@@ -3434,19 +3434,19 @@
     </row>
     <row r="25" spans="1:134" ht="15.75" customHeight="1">
       <c r="A25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="6"/>
@@ -3499,19 +3499,19 @@
     </row>
     <row r="26" spans="1:134" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="6"/>
@@ -3564,19 +3564,19 @@
     </row>
     <row r="27" spans="1:134" ht="15.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="6"/>
@@ -3629,19 +3629,19 @@
     </row>
     <row r="28" spans="1:134" ht="15.75" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="6"/>
@@ -3694,19 +3694,19 @@
     </row>
     <row r="29" spans="1:134" ht="15.75" customHeight="1">
       <c r="A29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="E29" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="1"/>
@@ -3759,19 +3759,19 @@
     </row>
     <row r="30" spans="1:134" ht="15.75" customHeight="1">
       <c r="A30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="1"/>
@@ -3824,19 +3824,19 @@
     </row>
     <row r="31" spans="1:134" ht="17.25" customHeight="1">
       <c r="A31" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="D31" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -3969,319 +3969,319 @@
     </row>
     <row r="32" spans="1:134" ht="15.75" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="C33" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="E35" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="E37" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B38" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="E38" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1">
       <c r="A39" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="12" t="s">
+      <c r="E40" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1">
       <c r="A43" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C43" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1">
       <c r="A44" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1">
       <c r="A45" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1">
       <c r="A47" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="12" t="s">
+      <c r="E47" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1">
       <c r="A48" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="E48" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1">
       <c r="A49" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J49" s="7"/>
     </row>

</xml_diff>